<commit_message>
Graph from 2010 to 2025
</commit_message>
<xml_diff>
--- a/api/data/calculator/data.xlsx
+++ b/api/data/calculator/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo Villalpando\Documents\MEXICOVID\mexicovid-19.app\api\data\calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE546C50-168C-4B66-93AC-6B3F4AB218C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73173994-9B52-4E0B-B5D9-958EEAEA0107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2712749A-A345-401B-A09A-6442F6619F7C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{2712749A-A345-401B-A09A-6442F6619F7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F422E72E-1F9E-40CE-A8CF-E57C3D67868E}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -729,10 +729,15 @@
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="3" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.42578125" style="1"/>
-    <col min="13" max="16384" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -1476,31 +1481,31 @@
       </c>
       <c r="C18" s="7">
         <f>C12*(1+$O$18)</f>
-        <v>11071292.445773419</v>
+        <v>10936567.929329811</v>
       </c>
       <c r="D18" s="7">
         <f>D12*(1+$N$18)</f>
-        <v>2194573.9909999999</v>
-      </c>
-      <c r="E18" s="7">
+        <v>2370748.91</v>
+      </c>
+      <c r="E18" s="12">
         <f>E12*(1+$O$18)</f>
-        <v>3163192.5110911406</v>
+        <v>3124700.2046542815</v>
       </c>
       <c r="F18" s="7">
         <f>F12*(1+$O$18)</f>
-        <v>86582.385745714288</v>
+        <v>85528.780657667114</v>
       </c>
       <c r="G18" s="7">
         <f>G12*(1+$O$18)</f>
-        <v>36801.365865449137</v>
+        <v>36353.536829681987</v>
       </c>
       <c r="H18" s="7">
         <f>H12*(1+$O$18)</f>
-        <v>119704.50052427842</v>
+        <v>118247.8385285587</v>
       </c>
       <c r="I18" s="8">
         <f t="shared" ref="I18" si="7">C18/($C18+$E18+$F18+$H18)</f>
-        <v>0.76666902337612552</v>
+        <v>0.76666902337612541</v>
       </c>
       <c r="J18" s="8">
         <f t="shared" ref="J18" si="8">E18/($C18+$E18+$F18+$H18)</f>
@@ -1508,21 +1513,21 @@
       </c>
       <c r="K18" s="8">
         <f t="shared" ref="K18" si="9">F18/($C18+$E18+$F18+$H18)</f>
-        <v>5.9956896131474705E-3</v>
+        <v>5.9956896131474714E-3</v>
       </c>
       <c r="L18" s="16">
         <f t="shared" ref="L18" si="10">H18/($C18+$E18+$F18+$H18)</f>
-        <v>8.2893422750937289E-3</v>
+        <v>8.2893422750937272E-3</v>
       </c>
       <c r="M18" s="9">
         <v>-0.1</v>
       </c>
       <c r="N18" s="10">
-        <v>8.9999999999999993E-3</v>
+        <v>0.09</v>
       </c>
       <c r="O18" s="11">
         <f>(B18-D18)/(B12-D12)-1</f>
-        <v>-0.11450034009987631</v>
+        <v>-0.12527582219244504</v>
       </c>
       <c r="P18" s="29"/>
       <c r="Q18" s="29"/>
@@ -1530,7 +1535,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="26"/>
-      <c r="B19" s="29"/>
+      <c r="B19" s="34">
+        <f>SUM(C18:H18)</f>
+        <v>16672147.200000001</v>
+      </c>
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
@@ -1714,31 +1722,31 @@
       </c>
       <c r="C25" s="36">
         <f t="shared" si="15"/>
-        <v>11071292.445773419</v>
+        <v>10936567.929329811</v>
       </c>
       <c r="D25" s="36">
         <f t="shared" si="15"/>
-        <v>2194573.9909999999</v>
+        <v>2370748.91</v>
       </c>
       <c r="E25" s="36">
         <f t="shared" si="15"/>
-        <v>3163192.5110911406</v>
+        <v>3124700.2046542815</v>
       </c>
       <c r="F25" s="36">
         <f t="shared" si="15"/>
-        <v>86582.385745714288</v>
+        <v>85528.780657667114</v>
       </c>
       <c r="G25" s="36">
         <f t="shared" si="15"/>
-        <v>36801.365865449137</v>
+        <v>36353.536829681987</v>
       </c>
       <c r="H25" s="36">
         <f t="shared" si="15"/>
-        <v>119704.50052427842</v>
+        <v>118247.8385285587</v>
       </c>
       <c r="I25" s="30">
         <f t="shared" si="12"/>
-        <v>0.76666902337612552</v>
+        <v>0.76666902337612541</v>
       </c>
       <c r="J25" s="30">
         <f t="shared" si="13"/>
@@ -1746,11 +1754,11 @@
       </c>
       <c r="K25" s="30">
         <f t="shared" si="13"/>
-        <v>5.9956896131474705E-3</v>
+        <v>5.9956896131474714E-3</v>
       </c>
       <c r="L25" s="31">
         <f t="shared" si="14"/>
-        <v>8.2893422750937289E-3</v>
+        <v>8.2893422750937272E-3</v>
       </c>
       <c r="M25" s="30"/>
       <c r="N25" s="30"/>
@@ -1765,31 +1773,31 @@
       </c>
       <c r="B26" s="12">
         <f>SUM(C26:H26)</f>
-        <v>16684151.696418928</v>
+        <v>16684151.696418926</v>
       </c>
       <c r="C26" s="12">
         <f>$C$25+($Q$21/$P$21)*($R$21-1)*I25</f>
-        <v>11073416.324745486</v>
+        <v>10938691.808301877</v>
       </c>
       <c r="D26" s="12">
         <f>D25+(Q21/P21)</f>
-        <v>2203808.2190145589</v>
+        <v>2379983.1380145592</v>
       </c>
       <c r="E26" s="12">
         <f>$E$25+($Q$21/$P$21)*($R$21-1)*J25</f>
-        <v>3163799.3271509465</v>
+        <v>3125307.0207140874</v>
       </c>
       <c r="F26" s="12">
         <f>$F$25+($Q$21/$P$21)*($R$21-1)*K25</f>
-        <v>86598.99541521199</v>
+        <v>85545.390327164816</v>
       </c>
       <c r="G26" s="12">
         <f>G25</f>
-        <v>36801.365865449137</v>
+        <v>36353.536829681987</v>
       </c>
       <c r="H26" s="13">
         <f>$H$25+($Q$21/$P$21)*($R$21-1)*L25</f>
-        <v>119727.46422727611</v>
+        <v>118270.80223155639</v>
       </c>
       <c r="I26" s="29"/>
       <c r="J26" s="29"/>
@@ -1797,7 +1805,7 @@
       <c r="L26" s="30"/>
       <c r="M26" s="33">
         <f>B26/B23-1</f>
-        <v>-9.935197028628473E-2</v>
+        <v>-9.9351970286284841E-2</v>
       </c>
       <c r="N26" s="29"/>
       <c r="O26" s="29"/>

</xml_diff>